<commit_message>
Update latest Daily Orders XLSX (2026-02-13 19:58:48)
</commit_message>
<xml_diff>
--- a/data/latest_daily_orders.xlsx
+++ b/data/latest_daily_orders.xlsx
@@ -556,19 +556,19 @@
         <v>اية</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>تم تأكيد الطلب</v>
       </c>
       <c r="D2" s="5">
         <v>46066.86900146991</v>
       </c>
       <c r="E2" s="5">
-        <v>46066.86906895833</v>
+        <v>46066.87028931713</v>
       </c>
       <c r="F2" s="4" t="str">
         <v>9647714219716</v>
       </c>
       <c r="G2" s="4" t="str">
-        <v>الجادرية</v>
+        <v>الجادرية-بغداد</v>
       </c>
       <c r="H2" s="4" t="str">
         <v>بغداد</v>

</xml_diff>

<commit_message>
Update latest Daily Orders XLSX (2026-02-15 22:57:11)
</commit_message>
<xml_diff>
--- a/data/latest_daily_orders.xlsx
+++ b/data/latest_daily_orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="الطلبات" sheetId="1" r:id="rId1"/>
+    <sheet name="Orders" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -479,73 +479,73 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
-        <v>رقم الطلب</v>
+        <v>ID</v>
       </c>
       <c r="B1" s="3" t="str">
-        <v>اسم المستلم</v>
+        <v>Customer Name</v>
       </c>
       <c r="C1" s="3" t="str">
-        <v>الحالة</v>
+        <v>Status</v>
       </c>
       <c r="D1" s="3" t="str">
-        <v>تاريخ الإنشاء</v>
+        <v>Created At</v>
       </c>
       <c r="E1" s="3" t="str">
-        <v>اخر تحديث</v>
+        <v>Updated At</v>
       </c>
       <c r="F1" s="3" t="str">
-        <v>رقم الهاتف</v>
+        <v>Phone Number</v>
       </c>
       <c r="G1" s="3" t="str">
-        <v>اسم الشارع</v>
+        <v>Street Name</v>
       </c>
       <c r="H1" s="3" t="str">
-        <v>المحافظة</v>
+        <v>Province</v>
       </c>
       <c r="I1" s="3" t="str">
         <v>orders.export.cashOnDelivery</v>
       </c>
       <c r="J1" s="3" t="str">
-        <v>تكلفة الشحن</v>
+        <v>Shipping Cost</v>
       </c>
       <c r="K1" s="3" t="str">
-        <v>ملاحظات</v>
+        <v>Notes</v>
       </c>
       <c r="L1" s="3" t="str">
-        <v>الدولة</v>
+        <v>Country</v>
       </c>
       <c r="M1" s="3" t="str">
-        <v>ربح الضريبة</v>
+        <v>VAT Profit</v>
       </c>
       <c r="N1" s="3" t="str">
-        <v>ربح الطلب</v>
+        <v>Order Profit</v>
       </c>
       <c r="O1" s="3" t="str">
-        <v>اسم الصفحة</v>
+        <v>Page Name</v>
       </c>
       <c r="P1" s="3" t="str">
-        <v>رابط الصفحة</v>
+        <v>Page URL</v>
       </c>
       <c r="Q1" s="3" t="str">
-        <v>المنتجات</v>
+        <v>SKUs</v>
       </c>
       <c r="R1" s="3" t="str">
-        <v>الكميات</v>
+        <v>Quantities</v>
       </c>
       <c r="S1" s="3" t="str">
-        <v>الأسعار</v>
+        <v>Prices</v>
       </c>
       <c r="T1" s="3" t="str">
-        <v>الطلب المستلم بواسطة</v>
+        <v>Order Received By</v>
       </c>
       <c r="U1" s="3" t="str">
-        <v>العنوان الوطني</v>
+        <v>National Address</v>
       </c>
       <c r="V1" s="3" t="str">
-        <v>مصدر العنوان الوطني</v>
+        <v>Source of the National Address</v>
       </c>
       <c r="W1" s="3" t="str">
-        <v>كود الطلب للمتجر</v>
+        <v>Store Order ID</v>
       </c>
     </row>
     <row r="2">
@@ -556,7 +556,7 @@
         <v>فاروق</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>Order Received</v>
       </c>
       <c r="D2" s="5">
         <v>46068.7900271875</v>
@@ -583,7 +583,7 @@
         <v/>
       </c>
       <c r="L2" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M2" s="4">
         <v>0</v>
@@ -627,7 +627,7 @@
         <v>Essam</v>
       </c>
       <c r="C3" s="4" t="str">
-        <v>تم تأكيد الطلب</v>
+        <v>Order Confirmed</v>
       </c>
       <c r="D3" s="5">
         <v>46068.6751509375</v>
@@ -654,7 +654,7 @@
         <v>please he order long time i need u to call him right now and say that stock to got it its was out of stock and give him the discount</v>
       </c>
       <c r="L3" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M3" s="4">
         <v>0</v>
@@ -698,7 +698,7 @@
         <v>يوسف علاء محمد</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D4" s="5">
         <v>46068.58809557871</v>
@@ -725,7 +725,7 @@
         <v/>
       </c>
       <c r="L4" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M4" s="4">
         <v>0</v>
@@ -769,7 +769,7 @@
         <v>مجيد خالد صالح</v>
       </c>
       <c r="C5" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>Order Received</v>
       </c>
       <c r="D5" s="5">
         <v>46068.56395737269</v>
@@ -796,7 +796,7 @@
         <v/>
       </c>
       <c r="L5" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M5" s="4">
         <v>0</v>
@@ -840,7 +840,7 @@
         <v>مايكل</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>تم تأكيد الطلب</v>
+        <v>Order Confirmed</v>
       </c>
       <c r="D6" s="5">
         <v>46068.56108516204</v>
@@ -867,7 +867,7 @@
         <v/>
       </c>
       <c r="L6" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>عمادحمدي</v>
       </c>
       <c r="C7" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D7" s="5">
         <v>46068.51948740741</v>
@@ -938,7 +938,7 @@
         <v/>
       </c>
       <c r="L7" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M7" s="4">
         <v>0</v>
@@ -982,7 +982,7 @@
         <v>مجتبى</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>تم تأكيد الطلب</v>
+        <v>Order Confirmed</v>
       </c>
       <c r="D8" s="5">
         <v>46068.51812688657</v>
@@ -1009,7 +1009,7 @@
         <v/>
       </c>
       <c r="L8" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M8" s="4">
         <v>0</v>
@@ -1053,7 +1053,7 @@
         <v>Muhammad</v>
       </c>
       <c r="C9" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>Order Received</v>
       </c>
       <c r="D9" s="5">
         <v>46068.51641268519</v>
@@ -1080,7 +1080,7 @@
         <v/>
       </c>
       <c r="L9" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M9" s="4">
         <v>0</v>
@@ -1124,7 +1124,7 @@
         <v>كرار</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D10" s="5">
         <v>46068.434168368054</v>
@@ -1151,7 +1151,7 @@
         <v/>
       </c>
       <c r="L10" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
@@ -1195,7 +1195,7 @@
         <v>نواف علي غالب</v>
       </c>
       <c r="C11" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D11" s="5">
         <v>46068.431902233795</v>
@@ -1222,7 +1222,7 @@
         <v/>
       </c>
       <c r="L11" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M11" s="4">
         <v>0</v>
@@ -1266,7 +1266,7 @@
         <v>فواز الصافي</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D12" s="5">
         <v>46068.43064762731</v>
@@ -1293,7 +1293,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L12" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M12" s="4">
         <v>0</v>
@@ -1337,7 +1337,7 @@
         <v>أبو الحب</v>
       </c>
       <c r="C13" s="4" t="str">
-        <v>في انتظار الشحن</v>
+        <v>Pending Shipping</v>
       </c>
       <c r="D13" s="5">
         <v>46068.39257596065</v>
@@ -1364,7 +1364,7 @@
         <v/>
       </c>
       <c r="L13" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M13" s="4">
         <v>0</v>
@@ -1408,13 +1408,13 @@
         <v>حقي اسماعيل كريم</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>في انتظار الشحن</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D14" s="5">
         <v>46068.39134778935</v>
       </c>
       <c r="E14" s="5">
-        <v>46068.84916466435</v>
+        <v>46068.927126145834</v>
       </c>
       <c r="F14" s="4" t="str">
         <v>9647803467635</v>
@@ -1435,7 +1435,7 @@
         <v/>
       </c>
       <c r="L14" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M14" s="4">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>انمار</v>
       </c>
       <c r="C15" s="4" t="str">
-        <v>في انتظار الشحن</v>
+        <v>Pending Shipping</v>
       </c>
       <c r="D15" s="5">
         <v>46068.38263501157</v>
@@ -1506,7 +1506,7 @@
         <v/>
       </c>
       <c r="L15" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M15" s="4">
         <v>0</v>
@@ -1550,7 +1550,7 @@
         <v>حيدر باسم علي</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>في انتظار الشحن</v>
+        <v>Pending Shipping</v>
       </c>
       <c r="D16" s="5">
         <v>46068.381668368056</v>
@@ -1577,7 +1577,7 @@
         <v/>
       </c>
       <c r="L16" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M16" s="4">
         <v>0</v>
@@ -1621,7 +1621,7 @@
         <v>علي امين كاطع</v>
       </c>
       <c r="C17" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D17" s="5">
         <v>46068.38064605324</v>
@@ -1648,7 +1648,7 @@
         <v/>
       </c>
       <c r="L17" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M17" s="4">
         <v>0</v>
@@ -1692,13 +1692,13 @@
         <v>عباس فاضل</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>في انتظار الشحن</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D18" s="5">
         <v>46068.37937023148</v>
       </c>
       <c r="E18" s="5">
-        <v>46068.849168692126</v>
+        <v>46068.92732148148</v>
       </c>
       <c r="F18" s="4" t="str">
         <v>9647711980896</v>
@@ -1719,7 +1719,7 @@
         <v/>
       </c>
       <c r="L18" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M18" s="4">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>محمد</v>
       </c>
       <c r="C19" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>Order Received</v>
       </c>
       <c r="D19" s="5">
         <v>46068.37652810185</v>
@@ -1790,7 +1790,7 @@
         <v/>
       </c>
       <c r="L19" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M19" s="4">
         <v>0</v>
@@ -1834,7 +1834,7 @@
         <v>ابو هاشم</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D20" s="5">
         <v>46067.92089087963</v>
@@ -1861,7 +1861,7 @@
         <v/>
       </c>
       <c r="L20" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M20" s="4">
         <v>0</v>
@@ -1905,7 +1905,7 @@
         <v>خالد</v>
       </c>
       <c r="C21" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D21" s="5">
         <v>46067.82353045139</v>
@@ -1932,7 +1932,7 @@
         <v/>
       </c>
       <c r="L21" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M21" s="4">
         <v>0</v>
@@ -1976,7 +1976,7 @@
         <v>ستيفن</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D22" s="5">
         <v>46067.77955053241</v>
@@ -2003,7 +2003,7 @@
         <v>call him asap please ordered 2 hours ago</v>
       </c>
       <c r="L22" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M22" s="4">
         <v>0</v>
@@ -2047,7 +2047,7 @@
         <v>علي حسن</v>
       </c>
       <c r="C23" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D23" s="5">
         <v>46067.609324502315</v>
@@ -2074,7 +2074,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L23" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M23" s="4">
         <v>0</v>
@@ -2118,7 +2118,7 @@
         <v>حسين</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D24" s="5">
         <v>46067.482777881945</v>
@@ -2145,7 +2145,7 @@
         <v/>
       </c>
       <c r="L24" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M24" s="4">
         <v>0</v>
@@ -2189,7 +2189,7 @@
         <v>علي عقيل</v>
       </c>
       <c r="C25" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>Order Received</v>
       </c>
       <c r="D25" s="5">
         <v>46067.44914142361</v>
@@ -2216,7 +2216,7 @@
         <v>call him asap please he orderd 3 hours ago</v>
       </c>
       <c r="L25" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M25" s="4">
         <v>0</v>
@@ -2260,7 +2260,7 @@
         <v>حسام الكعبي</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D26" s="5">
         <v>46067.366074502315</v>
@@ -2287,7 +2287,7 @@
         <v/>
       </c>
       <c r="L26" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M26" s="4">
         <v>0</v>
@@ -2331,7 +2331,7 @@
         <v>Mohammed</v>
       </c>
       <c r="C27" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D27" s="5">
         <v>46067.36500974537</v>
@@ -2358,7 +2358,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L27" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M27" s="4">
         <v>0</v>
@@ -2402,7 +2402,7 @@
         <v>Ammar</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D28" s="5">
         <v>46067.36414993055</v>
@@ -2429,7 +2429,7 @@
         <v/>
       </c>
       <c r="L28" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M28" s="4">
         <v>0</v>
@@ -2473,7 +2473,7 @@
         <v>علي أدم</v>
       </c>
       <c r="C29" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D29" s="5">
         <v>46067.075364525466</v>
@@ -2500,7 +2500,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L29" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M29" s="4">
         <v>0</v>
@@ -2544,7 +2544,7 @@
         <v>زيد</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D30" s="5">
         <v>46067.06385640046</v>
@@ -2571,7 +2571,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L30" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M30" s="4">
         <v>0</v>
@@ -2615,7 +2615,7 @@
         <v>عماد</v>
       </c>
       <c r="C31" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D31" s="5">
         <v>46067.02662810185</v>
@@ -2642,7 +2642,7 @@
         <v/>
       </c>
       <c r="L31" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M31" s="4">
         <v>0</v>
@@ -2686,7 +2686,7 @@
         <v>Danar dana</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D32" s="5">
         <v>46067.02529385417</v>
@@ -2713,7 +2713,7 @@
         <v/>
       </c>
       <c r="L32" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M32" s="4">
         <v>0</v>
@@ -2757,7 +2757,7 @@
         <v>ثامر</v>
       </c>
       <c r="C33" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D33" s="5">
         <v>46067.014509849534</v>
@@ -2784,7 +2784,7 @@
         <v/>
       </c>
       <c r="L33" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M33" s="4">
         <v>0</v>
@@ -2828,7 +2828,7 @@
         <v>Lawko sndi</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>تم تأكيد الطلب</v>
+        <v>Order Confirmed</v>
       </c>
       <c r="D34" s="5">
         <v>46066.93626458333</v>
@@ -2855,7 +2855,7 @@
         <v/>
       </c>
       <c r="L34" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M34" s="4">
         <v>0</v>
@@ -2899,7 +2899,7 @@
         <v>yahya</v>
       </c>
       <c r="C35" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D35" s="5">
         <v>46066.9186940162</v>
@@ -2926,7 +2926,7 @@
         <v>test</v>
       </c>
       <c r="L35" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M35" s="4">
         <v>0</v>
@@ -2970,7 +2970,7 @@
         <v>اية</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D36" s="5">
         <v>46066.86900146991</v>
@@ -2997,7 +2997,7 @@
         <v/>
       </c>
       <c r="L36" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M36" s="4">
         <v>0</v>
@@ -3041,7 +3041,7 @@
         <v>مؤمن</v>
       </c>
       <c r="C37" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D37" s="5">
         <v>46066.626790277776</v>
@@ -3068,7 +3068,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L37" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M37" s="4">
         <v>0</v>
@@ -3112,7 +3112,7 @@
         <v>مؤمن</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D38" s="5">
         <v>46066.62668688657</v>
@@ -3139,7 +3139,7 @@
         <v/>
       </c>
       <c r="L38" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M38" s="4">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         <v>حيدر انور</v>
       </c>
       <c r="C39" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D39" s="5">
         <v>46066.55861363426</v>
@@ -3210,7 +3210,7 @@
         <v/>
       </c>
       <c r="L39" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M39" s="4">
         <v>0</v>
@@ -3254,7 +3254,7 @@
         <v>عباس</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D40" s="5">
         <v>46066.43902012731</v>
@@ -3281,7 +3281,7 @@
         <v/>
       </c>
       <c r="L40" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M40" s="4">
         <v>0</v>
@@ -3325,7 +3325,7 @@
         <v>محمد مانع</v>
       </c>
       <c r="C41" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D41" s="5">
         <v>46066.437072395835</v>
@@ -3352,7 +3352,7 @@
         <v/>
       </c>
       <c r="L41" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M41" s="4">
         <v>0</v>
@@ -3396,7 +3396,7 @@
         <v>حسن</v>
       </c>
       <c r="C42" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D42" s="5">
         <v>46066.03705931713</v>
@@ -3423,7 +3423,7 @@
         <v/>
       </c>
       <c r="L42" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M42" s="4">
         <v>0</v>
@@ -3467,7 +3467,7 @@
         <v>Omar</v>
       </c>
       <c r="C43" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D43" s="5">
         <v>46065.998907002315</v>
@@ -3494,7 +3494,7 @@
         <v/>
       </c>
       <c r="L43" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M43" s="4">
         <v>0</v>
@@ -3538,7 +3538,7 @@
         <v>Rabih</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D44" s="5">
         <v>46065.984579930555</v>
@@ -3565,7 +3565,7 @@
         <v/>
       </c>
       <c r="L44" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M44" s="4">
         <v>0</v>
@@ -3609,7 +3609,7 @@
         <v>علي حسن</v>
       </c>
       <c r="C45" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D45" s="5">
         <v>46065.715770613424</v>
@@ -3636,7 +3636,7 @@
         <v/>
       </c>
       <c r="L45" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M45" s="4">
         <v>0</v>
@@ -3680,7 +3680,7 @@
         <v>عبدالكريم علي</v>
       </c>
       <c r="C46" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D46" s="5">
         <v>46065.51994837963</v>
@@ -3707,7 +3707,7 @@
         <v/>
       </c>
       <c r="L46" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M46" s="4">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>wwid</v>
       </c>
       <c r="C47" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D47" s="5">
         <v>46065.46910805556</v>
@@ -3778,7 +3778,7 @@
         <v/>
       </c>
       <c r="L47" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M47" s="4">
         <v>0</v>
@@ -3822,7 +3822,7 @@
         <v>وحده</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D48" s="5">
         <v>46065.12183098379</v>
@@ -3849,7 +3849,7 @@
         <v>no region no adress call him to check</v>
       </c>
       <c r="L48" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M48" s="4">
         <v>0</v>
@@ -3893,7 +3893,7 @@
         <v>علي رشدي</v>
       </c>
       <c r="C49" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D49" s="5">
         <v>46065.016198032405</v>
@@ -3920,7 +3920,7 @@
         <v/>
       </c>
       <c r="L49" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M49" s="4">
         <v>0</v>
@@ -3964,7 +3964,7 @@
         <v>احمد</v>
       </c>
       <c r="C50" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D50" s="5">
         <v>46065.01485634259</v>
@@ -3991,7 +3991,7 @@
         <v/>
       </c>
       <c r="L50" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M50" s="4">
         <v>0</v>
@@ -4035,7 +4035,7 @@
         <v>نجف</v>
       </c>
       <c r="C51" s="4" t="str">
-        <v>تم استلام الطلب</v>
+        <v>Order Received</v>
       </c>
       <c r="D51" s="5">
         <v>46064.66099334491</v>
@@ -4062,7 +4062,7 @@
         <v/>
       </c>
       <c r="L51" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M51" s="4">
         <v>0</v>
@@ -4106,7 +4106,7 @@
         <v>محمد جواد</v>
       </c>
       <c r="C52" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D52" s="5">
         <v>46064.62876076389</v>
@@ -4133,7 +4133,7 @@
         <v/>
       </c>
       <c r="L52" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M52" s="4">
         <v>0</v>
@@ -4177,7 +4177,7 @@
         <v>علي</v>
       </c>
       <c r="C53" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D53" s="5">
         <v>46064.58881206019</v>
@@ -4204,7 +4204,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L53" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M53" s="4">
         <v>0</v>
@@ -4248,7 +4248,7 @@
         <v>علي</v>
       </c>
       <c r="C54" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D54" s="5">
         <v>46064.58344008102</v>
@@ -4275,7 +4275,7 @@
         <v/>
       </c>
       <c r="L54" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M54" s="4">
         <v>0</v>
@@ -4319,7 +4319,7 @@
         <v>غيث عبد الرسول</v>
       </c>
       <c r="C55" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D55" s="5">
         <v>46064.57533837963</v>
@@ -4346,7 +4346,7 @@
         <v/>
       </c>
       <c r="L55" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M55" s="4">
         <v>0</v>
@@ -4390,7 +4390,7 @@
         <v>مؤمن طه حامد</v>
       </c>
       <c r="C56" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D56" s="5">
         <v>46064.57294252315</v>
@@ -4417,7 +4417,7 @@
         <v/>
       </c>
       <c r="L56" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M56" s="4">
         <v>0</v>
@@ -4461,7 +4461,7 @@
         <v>مصطفى</v>
       </c>
       <c r="C57" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D57" s="5">
         <v>46064.10276320602</v>
@@ -4488,7 +4488,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L57" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M57" s="4">
         <v>0</v>
@@ -4532,7 +4532,7 @@
         <v>مصطفى</v>
       </c>
       <c r="C58" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D58" s="5">
         <v>46064.10185199074</v>
@@ -4559,7 +4559,7 @@
         <v>call him as soon as possible he ordered 1h ago</v>
       </c>
       <c r="L58" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M58" s="4">
         <v>0</v>
@@ -4603,7 +4603,7 @@
         <v>ختام</v>
       </c>
       <c r="C59" s="4" t="str">
-        <v>فشل التسليم</v>
+        <v>Delivery Failed</v>
       </c>
       <c r="D59" s="5">
         <v>46064.05801408565</v>
@@ -4630,7 +4630,7 @@
         <v/>
       </c>
       <c r="L59" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M59" s="4">
         <v>0</v>
@@ -4674,7 +4674,7 @@
         <v>بدر</v>
       </c>
       <c r="C60" s="4" t="str">
-        <v>فشل التسليم</v>
+        <v>Delivery Failed</v>
       </c>
       <c r="D60" s="5">
         <v>46064.004486655096</v>
@@ -4701,7 +4701,7 @@
         <v>this one im not sure if he meant to order 2 pieces please check out with him</v>
       </c>
       <c r="L60" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M60" s="4">
         <v>0</v>
@@ -4745,7 +4745,7 @@
         <v>همام محمد عدنان</v>
       </c>
       <c r="C61" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D61" s="5">
         <v>46063.98810440972</v>
@@ -4772,7 +4772,7 @@
         <v>please call him for the right adress</v>
       </c>
       <c r="L61" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M61" s="4">
         <v>0</v>
@@ -4816,7 +4816,7 @@
         <v>حمزة</v>
       </c>
       <c r="C62" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D62" s="5">
         <v>46063.98408190972</v>
@@ -4843,7 +4843,7 @@
         <v/>
       </c>
       <c r="L62" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M62" s="4">
         <v>0</v>
@@ -4887,7 +4887,7 @@
         <v>همام محمد عدنان</v>
       </c>
       <c r="C63" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D63" s="5">
         <v>46063.961482858795</v>
@@ -4914,7 +4914,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L63" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M63" s="4">
         <v>0</v>
@@ -4958,7 +4958,7 @@
         <v>همام محمد عدنان</v>
       </c>
       <c r="C64" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D64" s="5">
         <v>46063.96038298611</v>
@@ -4985,7 +4985,7 @@
         <v>wrong</v>
       </c>
       <c r="L64" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M64" s="4">
         <v>0</v>
@@ -5029,7 +5029,7 @@
         <v>حمزة</v>
       </c>
       <c r="C65" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D65" s="5">
         <v>46063.95675210648</v>
@@ -5056,7 +5056,7 @@
         <v>wrong</v>
       </c>
       <c r="L65" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M65" s="4">
         <v>0</v>
@@ -5100,7 +5100,7 @@
         <v>حسين</v>
       </c>
       <c r="C66" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D66" s="5">
         <v>46063.95060015046</v>
@@ -5127,7 +5127,7 @@
         <v/>
       </c>
       <c r="L66" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M66" s="4">
         <v>0</v>
@@ -5171,7 +5171,7 @@
         <v>حسين</v>
       </c>
       <c r="C67" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D67" s="5">
         <v>46063.948616712965</v>
@@ -5198,7 +5198,7 @@
         <v>wrong</v>
       </c>
       <c r="L67" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M67" s="4">
         <v>0</v>
@@ -5242,7 +5242,7 @@
         <v>علاء</v>
       </c>
       <c r="C68" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D68" s="5">
         <v>46063.849569907405</v>
@@ -5269,7 +5269,7 @@
         <v/>
       </c>
       <c r="L68" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M68" s="4">
         <v>0</v>
@@ -5313,7 +5313,7 @@
         <v>أدور</v>
       </c>
       <c r="C69" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D69" s="5">
         <v>46063.84274976852</v>
@@ -5340,7 +5340,7 @@
         <v>please call him he orderded 1h ago</v>
       </c>
       <c r="L69" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M69" s="4">
         <v>0</v>
@@ -5384,7 +5384,7 @@
         <v>رامي</v>
       </c>
       <c r="C70" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D70" s="5">
         <v>46063.74508501157</v>
@@ -5411,7 +5411,7 @@
         <v/>
       </c>
       <c r="L70" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M70" s="4">
         <v>0</v>
@@ -5455,7 +5455,7 @@
         <v>Lizan ahmed</v>
       </c>
       <c r="C71" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D71" s="5">
         <v>46063.669380127314</v>
@@ -5482,7 +5482,7 @@
         <v/>
       </c>
       <c r="L71" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M71" s="4">
         <v>0</v>
@@ -5526,7 +5526,7 @@
         <v>فرح</v>
       </c>
       <c r="C72" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D72" s="5">
         <v>46063.66798331019</v>
@@ -5553,7 +5553,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L72" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M72" s="4">
         <v>0</v>
@@ -5597,7 +5597,7 @@
         <v>فرح</v>
       </c>
       <c r="C73" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D73" s="5">
         <v>46063.667939756946</v>
@@ -5624,7 +5624,7 @@
         <v/>
       </c>
       <c r="L73" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M73" s="4">
         <v>0</v>
@@ -5668,7 +5668,7 @@
         <v>Ako</v>
       </c>
       <c r="C74" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D74" s="5">
         <v>46063.50018960648</v>
@@ -5695,7 +5695,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L74" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M74" s="4">
         <v>0</v>
@@ -5739,7 +5739,7 @@
         <v>A Talabany</v>
       </c>
       <c r="C75" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D75" s="5">
         <v>46063.494396145834</v>
@@ -5767,7 +5767,7 @@
         <v>call him asap he ordered 40 min ago</v>
       </c>
       <c r="L75" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M75" s="4">
         <v>0</v>
@@ -5811,7 +5811,7 @@
         <v>حيدر</v>
       </c>
       <c r="C76" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D76" s="5">
         <v>46063.363034456015</v>
@@ -5838,7 +5838,7 @@
         <v/>
       </c>
       <c r="L76" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M76" s="4">
         <v>0</v>
@@ -5882,7 +5882,7 @@
         <v>وسام</v>
       </c>
       <c r="C77" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D77" s="5">
         <v>46063.36197258102</v>
@@ -5910,7 +5910,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L77" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M77" s="4">
         <v>0</v>
@@ -5954,7 +5954,7 @@
         <v>سيفر سردار</v>
       </c>
       <c r="C78" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D78" s="5">
         <v>46062.94732335648</v>
@@ -5981,7 +5981,7 @@
         <v/>
       </c>
       <c r="L78" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M78" s="4">
         <v>0</v>
@@ -6025,7 +6025,7 @@
         <v>Saja</v>
       </c>
       <c r="C79" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D79" s="5">
         <v>46062.79384813657</v>
@@ -6052,7 +6052,7 @@
         <v/>
       </c>
       <c r="L79" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M79" s="4">
         <v>0</v>
@@ -6096,7 +6096,7 @@
         <v>عباس</v>
       </c>
       <c r="C80" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D80" s="5">
         <v>46062.79220025463</v>
@@ -6123,7 +6123,7 @@
         <v/>
       </c>
       <c r="L80" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M80" s="4">
         <v>0</v>
@@ -6167,7 +6167,7 @@
         <v>برهيم علي سجاد</v>
       </c>
       <c r="C81" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D81" s="5">
         <v>46062.64360072916</v>
@@ -6194,7 +6194,7 @@
         <v/>
       </c>
       <c r="L81" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M81" s="4">
         <v>0</v>
@@ -6238,7 +6238,7 @@
         <v>علي جبار</v>
       </c>
       <c r="C82" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D82" s="5">
         <v>46062.64234420139</v>
@@ -6265,7 +6265,7 @@
         <v/>
       </c>
       <c r="L82" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M82" s="4">
         <v>0</v>
@@ -6309,7 +6309,7 @@
         <v>اسيل</v>
       </c>
       <c r="C83" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D83" s="5">
         <v>46062.5843108912</v>
@@ -6336,7 +6336,7 @@
         <v>discount number</v>
       </c>
       <c r="L83" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M83" s="4">
         <v>0</v>
@@ -6380,7 +6380,7 @@
         <v>فهد</v>
       </c>
       <c r="C84" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D84" s="5">
         <v>46062.54285048611</v>
@@ -6407,7 +6407,7 @@
         <v/>
       </c>
       <c r="L84" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M84" s="4">
         <v>0</v>
@@ -6451,7 +6451,7 @@
         <v>Samer sabah</v>
       </c>
       <c r="C85" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D85" s="5">
         <v>46062.50750659722</v>
@@ -6478,7 +6478,7 @@
         <v/>
       </c>
       <c r="L85" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M85" s="4">
         <v>0</v>
@@ -6522,7 +6522,7 @@
         <v>Mohammed I</v>
       </c>
       <c r="C86" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D86" s="5">
         <v>46062.45230179398</v>
@@ -6549,7 +6549,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L86" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M86" s="4">
         <v>0</v>
@@ -6593,7 +6593,7 @@
         <v>Mohammed I</v>
       </c>
       <c r="C87" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D87" s="5">
         <v>46062.451287627315</v>
@@ -6620,7 +6620,7 @@
         <v>wrong</v>
       </c>
       <c r="L87" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M87" s="4">
         <v>0</v>
@@ -6664,7 +6664,7 @@
         <v>Mohammed abdulzahra</v>
       </c>
       <c r="C88" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D88" s="5">
         <v>46062.42305118056</v>
@@ -6691,7 +6691,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L88" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M88" s="4">
         <v>0</v>
@@ -6735,7 +6735,7 @@
         <v>Mohammed I</v>
       </c>
       <c r="C89" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D89" s="5">
         <v>46062.413627974536</v>
@@ -6762,7 +6762,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L89" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M89" s="4">
         <v>0</v>
@@ -6806,7 +6806,7 @@
         <v>Mohammed abdulzahra</v>
       </c>
       <c r="C90" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D90" s="5">
         <v>46062.41033025463</v>
@@ -6833,7 +6833,7 @@
         <v/>
       </c>
       <c r="L90" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M90" s="4">
         <v>0</v>
@@ -6877,7 +6877,7 @@
         <v>علي الرجب</v>
       </c>
       <c r="C91" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D91" s="5">
         <v>46062.409052650466</v>
@@ -6904,7 +6904,7 @@
         <v/>
       </c>
       <c r="L91" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M91" s="4">
         <v>0</v>
@@ -6948,7 +6948,7 @@
         <v>خالد كاظم</v>
       </c>
       <c r="C92" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D92" s="5">
         <v>46062.39857081018</v>
@@ -6975,7 +6975,7 @@
         <v/>
       </c>
       <c r="L92" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M92" s="4">
         <v>0</v>
@@ -7019,7 +7019,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C93" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D93" s="5">
         <v>46062.12001951389</v>
@@ -7046,7 +7046,7 @@
         <v>duplucated</v>
       </c>
       <c r="L93" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M93" s="4">
         <v>0</v>
@@ -7090,7 +7090,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C94" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D94" s="5">
         <v>46062.11975269676</v>
@@ -7117,7 +7117,7 @@
         <v>duplucated</v>
       </c>
       <c r="L94" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M94" s="4">
         <v>0</v>
@@ -7161,7 +7161,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C95" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D95" s="5">
         <v>46062.119456875</v>
@@ -7188,7 +7188,7 @@
         <v>duplucated</v>
       </c>
       <c r="L95" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M95" s="4">
         <v>0</v>
@@ -7232,7 +7232,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C96" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D96" s="5">
         <v>46062.119129618055</v>
@@ -7259,7 +7259,7 @@
         <v>duplucated</v>
       </c>
       <c r="L96" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M96" s="4">
         <v>0</v>
@@ -7303,7 +7303,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C97" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D97" s="5">
         <v>46062.1181390162</v>
@@ -7330,7 +7330,7 @@
         <v>كردي و مفيش واتساب</v>
       </c>
       <c r="L97" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M97" s="4">
         <v>0</v>
@@ -7374,7 +7374,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C98" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D98" s="5">
         <v>46062.116491030094</v>
@@ -7401,7 +7401,7 @@
         <v/>
       </c>
       <c r="L98" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M98" s="4">
         <v>0</v>
@@ -7445,7 +7445,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C99" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D99" s="5">
         <v>46062.11577030092</v>
@@ -7472,7 +7472,7 @@
         <v>duplucated</v>
       </c>
       <c r="L99" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M99" s="4">
         <v>0</v>
@@ -7516,7 +7516,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C100" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D100" s="5">
         <v>46062.1151934375</v>
@@ -7543,7 +7543,7 @@
         <v>duplucated</v>
       </c>
       <c r="L100" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M100" s="4">
         <v>0</v>
@@ -7587,7 +7587,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C101" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D101" s="5">
         <v>46062.114325393515</v>
@@ -7614,7 +7614,7 @@
         <v>duplucated</v>
       </c>
       <c r="L101" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M101" s="4">
         <v>0</v>
@@ -7658,7 +7658,7 @@
         <v>حسين</v>
       </c>
       <c r="C102" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D102" s="5">
         <v>46062.05659570602</v>
@@ -7685,7 +7685,7 @@
         <v/>
       </c>
       <c r="L102" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M102" s="4">
         <v>0</v>
@@ -7729,7 +7729,7 @@
         <v>فارس</v>
       </c>
       <c r="C103" s="4" t="str">
-        <v>قيد التوصيل</v>
+        <v>Delivery in Progress</v>
       </c>
       <c r="D103" s="5">
         <v>46062.03247658565</v>
@@ -7756,7 +7756,7 @@
         <v/>
       </c>
       <c r="L103" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M103" s="4">
         <v>0</v>
@@ -7800,7 +7800,7 @@
         <v>مجيد</v>
       </c>
       <c r="C104" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D104" s="5">
         <v>46062.031249328706</v>
@@ -7827,7 +7827,7 @@
         <v>this one didn't order quantity two he ordered first time then second time please confirm with him if he meant 1 or 2</v>
       </c>
       <c r="L104" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M104" s="4">
         <v>0</v>
@@ -7871,7 +7871,7 @@
         <v>اركان</v>
       </c>
       <c r="C105" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D105" s="5">
         <v>46062.02948613426</v>
@@ -7898,7 +7898,7 @@
         <v/>
       </c>
       <c r="L105" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M105" s="4">
         <v>0</v>
@@ -7942,7 +7942,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C106" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D106" s="5">
         <v>46061.87229554398</v>
@@ -7969,7 +7969,7 @@
         <v>duplucated</v>
       </c>
       <c r="L106" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M106" s="4">
         <v>0</v>
@@ -8013,7 +8013,7 @@
         <v>علاء بديري</v>
       </c>
       <c r="C107" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D107" s="5">
         <v>46061.87095564815</v>
@@ -8040,7 +8040,7 @@
         <v>duplucated</v>
       </c>
       <c r="L107" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M107" s="4">
         <v>0</v>
@@ -8084,7 +8084,7 @@
         <v>Ulla</v>
       </c>
       <c r="C108" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D108" s="5">
         <v>46061.631386469904</v>
@@ -8111,7 +8111,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L108" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M108" s="4">
         <v>0</v>
@@ -8155,7 +8155,7 @@
         <v>عمر عبدالله</v>
       </c>
       <c r="C109" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D109" s="5">
         <v>46061.54547142361</v>
@@ -8182,7 +8182,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L109" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M109" s="4">
         <v>0</v>
@@ -8226,7 +8226,7 @@
         <v>Ulla</v>
       </c>
       <c r="C110" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D110" s="5">
         <v>46061.41131630787</v>
@@ -8253,7 +8253,7 @@
         <v/>
       </c>
       <c r="L110" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M110" s="4">
         <v>0</v>
@@ -8297,7 +8297,7 @@
         <v>يوسف</v>
       </c>
       <c r="C111" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D111" s="5">
         <v>46061.410177777776</v>
@@ -8324,7 +8324,7 @@
         <v/>
       </c>
       <c r="L111" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M111" s="4">
         <v>0</v>
@@ -8368,7 +8368,7 @@
         <v>زيد كامل</v>
       </c>
       <c r="C112" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D112" s="5">
         <v>46061.40806185185</v>
@@ -8395,7 +8395,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L112" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M112" s="4">
         <v>0</v>
@@ -8439,7 +8439,7 @@
         <v>حسين ستار</v>
       </c>
       <c r="C113" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D113" s="5">
         <v>46061.40700960648</v>
@@ -8466,7 +8466,7 @@
         <v/>
       </c>
       <c r="L113" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M113" s="4">
         <v>0</v>
@@ -8510,7 +8510,7 @@
         <v>سجاد</v>
       </c>
       <c r="C114" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D114" s="5">
         <v>46061.40609613426</v>
@@ -8537,7 +8537,7 @@
         <v/>
       </c>
       <c r="L114" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M114" s="4">
         <v>0</v>
@@ -8581,7 +8581,7 @@
         <v>Bashar</v>
       </c>
       <c r="C115" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D115" s="5">
         <v>46061.31099184028</v>
@@ -8608,7 +8608,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L115" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M115" s="4">
         <v>0</v>
@@ -8652,7 +8652,7 @@
         <v>عباس محمد اسماعيل</v>
       </c>
       <c r="C116" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D116" s="5">
         <v>46061.30975965278</v>
@@ -8679,7 +8679,7 @@
         <v/>
       </c>
       <c r="L116" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M116" s="4">
         <v>0</v>
@@ -8723,7 +8723,7 @@
         <v>Hadeeth</v>
       </c>
       <c r="C117" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D117" s="5">
         <v>46061.072884814814</v>
@@ -8750,7 +8750,7 @@
         <v/>
       </c>
       <c r="L117" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M117" s="4">
         <v>0</v>
@@ -8794,7 +8794,7 @@
         <v>سجاد</v>
       </c>
       <c r="C118" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D118" s="5">
         <v>46061.068113912035</v>
@@ -8821,7 +8821,7 @@
         <v/>
       </c>
       <c r="L118" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M118" s="4">
         <v>0</v>
@@ -8865,7 +8865,7 @@
         <v>حسن</v>
       </c>
       <c r="C119" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D119" s="5">
         <v>46061.059307511576</v>
@@ -8892,7 +8892,7 @@
         <v/>
       </c>
       <c r="L119" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M119" s="4">
         <v>0</v>
@@ -8936,7 +8936,7 @@
         <v>دعاء يحيى</v>
       </c>
       <c r="C120" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D120" s="5">
         <v>46061.0553649537</v>
@@ -8963,7 +8963,7 @@
         <v>duplicated</v>
       </c>
       <c r="L120" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M120" s="4">
         <v>0</v>
@@ -9007,7 +9007,7 @@
         <v>دعاء يحيى</v>
       </c>
       <c r="C121" s="4" t="str">
-        <v>تم التحقق من الإرجاع</v>
+        <v>Return Verified</v>
       </c>
       <c r="D121" s="5">
         <v>46061.05291396991</v>
@@ -9034,7 +9034,7 @@
         <v/>
       </c>
       <c r="L121" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M121" s="4">
         <v>0</v>
@@ -9078,7 +9078,7 @@
         <v>اوس</v>
       </c>
       <c r="C122" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D122" s="5">
         <v>46060.894264699076</v>
@@ -9105,7 +9105,7 @@
         <v>تم تأكيد الطلب تلقائيا لأن العميل استلم طلب سابق لنفس العنوان</v>
       </c>
       <c r="L122" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M122" s="4">
         <v>0</v>
@@ -9149,7 +9149,7 @@
         <v>عباس</v>
       </c>
       <c r="C123" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D123" s="5">
         <v>46060.892965555555</v>
@@ -9176,7 +9176,7 @@
         <v>call asap</v>
       </c>
       <c r="L123" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M123" s="4">
         <v>0</v>
@@ -9220,7 +9220,7 @@
         <v>قاسم</v>
       </c>
       <c r="C124" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D124" s="5">
         <v>46060.81830115741</v>
@@ -9247,7 +9247,7 @@
         <v>call asap</v>
       </c>
       <c r="L124" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M124" s="4">
         <v>0</v>
@@ -9291,7 +9291,7 @@
         <v>قاسم</v>
       </c>
       <c r="C125" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D125" s="5">
         <v>46060.81512138889</v>
@@ -9318,7 +9318,7 @@
         <v>wrong</v>
       </c>
       <c r="L125" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M125" s="4">
         <v>0</v>
@@ -9362,7 +9362,7 @@
         <v>ايمان</v>
       </c>
       <c r="C126" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D126" s="5">
         <v>46060.668517604165</v>
@@ -9389,7 +9389,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L126" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M126" s="4">
         <v>0</v>
@@ -9433,7 +9433,7 @@
         <v>جنان</v>
       </c>
       <c r="C127" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D127" s="5">
         <v>46060.62921245371</v>
@@ -9460,7 +9460,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L127" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M127" s="4">
         <v>0</v>
@@ -9504,7 +9504,7 @@
         <v>Marwa</v>
       </c>
       <c r="C128" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D128" s="5">
         <v>46060.624529305554</v>
@@ -9531,7 +9531,7 @@
         <v/>
       </c>
       <c r="L128" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M128" s="4">
         <v>0</v>
@@ -9575,7 +9575,7 @@
         <v>جنان</v>
       </c>
       <c r="C129" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D129" s="5">
         <v>46060.526294131945</v>
@@ -9602,7 +9602,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L129" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M129" s="4">
         <v>0</v>
@@ -9646,7 +9646,7 @@
         <v>Mazin</v>
       </c>
       <c r="C130" s="4" t="str">
-        <v>تم التحقق من الإرجاع</v>
+        <v>Return Verified</v>
       </c>
       <c r="D130" s="5">
         <v>46060.522677974535</v>
@@ -9673,7 +9673,7 @@
         <v>call asap</v>
       </c>
       <c r="L130" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M130" s="4">
         <v>0</v>
@@ -9717,7 +9717,7 @@
         <v>محمد</v>
       </c>
       <c r="C131" s="4" t="str">
-        <v>معلق مؤقتًا</v>
+        <v>Temporary Suspended</v>
       </c>
       <c r="D131" s="5">
         <v>46060.521560416666</v>
@@ -9744,7 +9744,7 @@
         <v/>
       </c>
       <c r="L131" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M131" s="4">
         <v>0</v>
@@ -9788,7 +9788,7 @@
         <v>علي</v>
       </c>
       <c r="C132" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D132" s="5">
         <v>46060.51972076389</v>
@@ -9815,7 +9815,7 @@
         <v>call asap</v>
       </c>
       <c r="L132" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M132" s="4">
         <v>0</v>
@@ -9859,7 +9859,7 @@
         <v>جنان</v>
       </c>
       <c r="C133" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D133" s="5">
         <v>46060.518487141206</v>
@@ -9886,7 +9886,7 @@
         <v>هذا الطلب مكرر</v>
       </c>
       <c r="L133" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M133" s="4">
         <v>0</v>
@@ -9930,7 +9930,7 @@
         <v>ايمان</v>
       </c>
       <c r="C134" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D134" s="5">
         <v>46060.51780462963</v>
@@ -9957,7 +9957,7 @@
         <v>call asap</v>
       </c>
       <c r="L134" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M134" s="4">
         <v>0</v>
@@ -10001,7 +10001,7 @@
         <v>كرار</v>
       </c>
       <c r="C135" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D135" s="5">
         <v>46060.51636940972</v>
@@ -10028,7 +10028,7 @@
         <v/>
       </c>
       <c r="L135" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M135" s="4">
         <v>0</v>
@@ -10072,7 +10072,7 @@
         <v>غادة</v>
       </c>
       <c r="C136" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D136" s="5">
         <v>46060.514743113425</v>
@@ -10099,7 +10099,7 @@
         <v/>
       </c>
       <c r="L136" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M136" s="4">
         <v>0</v>
@@ -10143,7 +10143,7 @@
         <v>عماد طارق عبد الجبار</v>
       </c>
       <c r="C137" s="4" t="str">
-        <v>تم التحقق من الإرجاع</v>
+        <v>Return Verified</v>
       </c>
       <c r="D137" s="5">
         <v>46060.51269715278</v>
@@ -10170,7 +10170,7 @@
         <v>call asap</v>
       </c>
       <c r="L137" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M137" s="4">
         <v>0</v>
@@ -10214,7 +10214,7 @@
         <v>غصون عبد الرحيم عاقل</v>
       </c>
       <c r="C138" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D138" s="5">
         <v>46060.509699305556</v>
@@ -10241,7 +10241,7 @@
         <v>call asap</v>
       </c>
       <c r="L138" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M138" s="4">
         <v>0</v>
@@ -10285,7 +10285,7 @@
         <v>د ريا عبد الامير</v>
       </c>
       <c r="C139" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D139" s="5">
         <v>46060.50026450231</v>
@@ -10312,7 +10312,7 @@
         <v/>
       </c>
       <c r="L139" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M139" s="4">
         <v>0</v>
@@ -10356,7 +10356,7 @@
         <v>علي</v>
       </c>
       <c r="C140" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D140" s="5">
         <v>46057.68370048611</v>
@@ -10384,7 +10384,7 @@
         <v>he did not put the full adress</v>
       </c>
       <c r="L140" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M140" s="4">
         <v>0</v>
@@ -10428,7 +10428,7 @@
         <v>مبننرمك</v>
       </c>
       <c r="C141" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D141" s="5">
         <v>46057.64231769676</v>
@@ -10455,7 +10455,7 @@
         <v/>
       </c>
       <c r="L141" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M141" s="4">
         <v>0</v>
@@ -10499,7 +10499,7 @@
         <v>مبننرمك</v>
       </c>
       <c r="C142" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D142" s="5">
         <v>46057.64010853009</v>
@@ -10526,7 +10526,7 @@
         <v>wrong</v>
       </c>
       <c r="L142" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M142" s="4">
         <v>0</v>
@@ -10570,7 +10570,7 @@
         <v>مبننرمك</v>
       </c>
       <c r="C143" s="4" t="str">
-        <v>طلب ملغي بواسطتك</v>
+        <v>Cancelled by You</v>
       </c>
       <c r="D143" s="5">
         <v>46057.635958113424</v>
@@ -10597,7 +10597,7 @@
         <v>wrong</v>
       </c>
       <c r="L143" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M143" s="4">
         <v>0</v>
@@ -10641,7 +10641,7 @@
         <v>Esam</v>
       </c>
       <c r="C144" s="4" t="str">
-        <v>تم التحقق من الإرجاع</v>
+        <v>Return Verified</v>
       </c>
       <c r="D144" s="5">
         <v>46057.626599282405</v>
@@ -10669,7 +10669,7 @@
         <v>get the right adress please</v>
       </c>
       <c r="L144" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M144" s="4">
         <v>0</v>
@@ -10713,7 +10713,7 @@
         <v>marwan jawad</v>
       </c>
       <c r="C145" s="4" t="str">
-        <v>تم التوصيل</v>
+        <v>Delivered</v>
       </c>
       <c r="D145" s="5">
         <v>46057.555198912036</v>
@@ -10741,7 +10741,7 @@
         <v>need to call him as soon as possible cuz we had an error</v>
       </c>
       <c r="L145" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M145" s="4">
         <v>0</v>
@@ -10785,7 +10785,7 @@
         <v>marwan jawad</v>
       </c>
       <c r="C146" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D146" s="5">
         <v>46057.548482673614</v>
@@ -10812,7 +10812,7 @@
         <v>مكرر</v>
       </c>
       <c r="L146" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M146" s="4">
         <v>0</v>
@@ -10856,7 +10856,7 @@
         <v>Test</v>
       </c>
       <c r="C147" s="4" t="str">
-        <v>العميل رفض التأكيد</v>
+        <v>Customer Rejected</v>
       </c>
       <c r="D147" s="5">
         <v>46009.94421743056</v>
@@ -10884,7 +10884,7 @@
 </v>
       </c>
       <c r="L147" s="4" t="str">
-        <v>العراق</v>
+        <v>Iraq</v>
       </c>
       <c r="M147" s="4">
         <v>0</v>

</xml_diff>